<commit_message>
Pre-vintaging configuration: - Deactivated passenger sector to test impact of vintage sets.
</commit_message>
<xml_diff>
--- a/data/zenodo/storage/CHE_sto_pumpedhydro.xlsx
+++ b/data/zenodo/storage/CHE_sto_pumpedhydro.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/zenodo_ivan/storage/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/zenodo/storage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFA43CC-CF02-4D49-8763-729811B0D7C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF9FB91-1D47-A74B-8A99-0CDE956A0FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10100" yWindow="500" windowWidth="21600" windowHeight="19900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$L$576</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$L$577</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1893" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="103">
   <si>
     <t>Name:</t>
   </si>
@@ -339,6 +339,9 @@
   </si>
   <si>
     <t>Maximum energy production per capacity unit, per year.</t>
+  </si>
+  <si>
+    <t>enable_year</t>
   </si>
 </sst>
 </file>
@@ -434,7 +437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -446,6 +449,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -785,11 +791,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L319"/>
+  <dimension ref="A1:L320"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12:L12"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -884,23 +890,20 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F7" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -911,7 +914,7 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D8" t="s">
         <v>99</v>
@@ -922,7 +925,6 @@
       <c r="G8">
         <v>1</v>
       </c>
-      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -932,10 +934,10 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F9" t="s">
         <v>44</v>
@@ -943,12 +945,7 @@
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="J9" t="s">
-        <v>46</v>
-      </c>
-      <c r="L9" t="s">
-        <v>56</v>
-      </c>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -958,7 +955,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
         <v>95</v>
@@ -967,91 +964,91 @@
         <v>44</v>
       </c>
       <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>46</v>
+      </c>
+      <c r="L10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11">
         <v>0.82</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J11" t="s">
         <v>53</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="4" t="s">
+    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11" t="s">
-        <v>47</v>
-      </c>
-      <c r="I11" t="s">
-        <v>45</v>
-      </c>
-      <c r="J11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>96</v>
       </c>
       <c r="D12" t="s">
         <v>24</v>
       </c>
       <c r="G12">
-        <v>31.54</v>
+        <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>100</v>
-      </c>
-      <c r="L12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="I12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>27</v>
+      <c r="C13" t="s">
+        <v>96</v>
       </c>
       <c r="D13" t="s">
         <v>24</v>
       </c>
       <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I13" t="s">
-        <v>45</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>46</v>
+        <v>31.54</v>
+      </c>
+      <c r="H13" t="s">
+        <v>100</v>
+      </c>
+      <c r="L13" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1062,21 +1059,23 @@
         <v>19</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
         <v>24</v>
       </c>
       <c r="G14">
-        <v>8.3000000000000007</v>
+        <v>0</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="I14" t="s">
         <v>45</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1086,16 +1085,19 @@
         <v>19</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
         <v>24</v>
       </c>
       <c r="G15">
-        <v>40</v>
-      </c>
-      <c r="H15" t="s">
-        <v>49</v>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="I15" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" t="s">
+        <v>46</v>
       </c>
       <c r="K15" s="3"/>
     </row>
@@ -1107,22 +1109,16 @@
         <v>19</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
         <v>24</v>
       </c>
       <c r="G16">
-        <v>2500</v>
+        <v>40</v>
       </c>
       <c r="H16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I16" t="s">
-        <v>45</v>
-      </c>
-      <c r="J16" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="K16" s="3"/>
     </row>
@@ -1134,49 +1130,52 @@
         <v>19</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
         <v>24</v>
       </c>
       <c r="G17">
+        <v>2500</v>
+      </c>
+      <c r="H17" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" t="s">
+        <v>46</v>
+      </c>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18">
         <f>1840*1.3</f>
         <v>2392</v>
       </c>
-      <c r="H17" t="s">
-        <v>51</v>
-      </c>
-      <c r="J17" t="s">
-        <v>46</v>
-      </c>
-      <c r="K17" s="3"/>
-      <c r="L17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18">
-        <v>0.9</v>
-      </c>
-      <c r="I18" t="s">
-        <v>45</v>
+      <c r="H18" t="s">
+        <v>51</v>
       </c>
       <c r="J18" t="s">
         <v>46</v>
       </c>
       <c r="K18" s="3"/>
+      <c r="L18" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -1186,50 +1185,42 @@
         <v>19</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" t="s">
         <v>24</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>0.9</v>
+      </c>
+      <c r="I19" t="s">
+        <v>45</v>
       </c>
       <c r="J19" t="s">
         <v>46</v>
       </c>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" t="s">
-        <v>34</v>
+      <c r="C20" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20">
-        <v>1990</v>
+        <v>24</v>
       </c>
       <c r="G20">
-        <v>1695</v>
-      </c>
-      <c r="H20" t="s">
-        <v>50</v>
-      </c>
-      <c r="I20" t="s">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>57</v>
-      </c>
-      <c r="L20" t="s">
-        <v>58</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -1245,10 +1236,10 @@
         <v>18</v>
       </c>
       <c r="E21">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="G21">
-        <v>1946</v>
+        <v>1695</v>
       </c>
       <c r="H21" t="s">
         <v>50</v>
@@ -1257,7 +1248,7 @@
         <v>45</v>
       </c>
       <c r="J21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L21" t="s">
         <v>58</v>
@@ -1277,10 +1268,10 @@
         <v>18</v>
       </c>
       <c r="E22">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="G22">
-        <v>1438</v>
+        <v>1946</v>
       </c>
       <c r="H22" t="s">
         <v>50</v>
@@ -1289,7 +1280,7 @@
         <v>45</v>
       </c>
       <c r="J22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L22" t="s">
         <v>58</v>
@@ -1309,10 +1300,10 @@
         <v>18</v>
       </c>
       <c r="E23">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="G23">
-        <v>1186</v>
+        <v>1438</v>
       </c>
       <c r="H23" t="s">
         <v>50</v>
@@ -1321,7 +1312,7 @@
         <v>45</v>
       </c>
       <c r="J23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L23" t="s">
         <v>58</v>
@@ -1341,10 +1332,10 @@
         <v>18</v>
       </c>
       <c r="E24">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="G24">
-        <v>1271</v>
+        <v>1186</v>
       </c>
       <c r="H24" t="s">
         <v>50</v>
@@ -1353,7 +1344,7 @@
         <v>45</v>
       </c>
       <c r="J24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L24" t="s">
         <v>58</v>
@@ -1373,10 +1364,10 @@
         <v>18</v>
       </c>
       <c r="E25">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="G25">
-        <v>1520</v>
+        <v>1271</v>
       </c>
       <c r="H25" t="s">
         <v>50</v>
@@ -1385,7 +1376,7 @@
         <v>45</v>
       </c>
       <c r="J25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L25" t="s">
         <v>58</v>
@@ -1405,10 +1396,10 @@
         <v>18</v>
       </c>
       <c r="E26">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="G26">
-        <v>1754</v>
+        <v>1520</v>
       </c>
       <c r="H26" t="s">
         <v>50</v>
@@ -1417,7 +1408,7 @@
         <v>45</v>
       </c>
       <c r="J26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L26" t="s">
         <v>58</v>
@@ -1437,10 +1428,10 @@
         <v>18</v>
       </c>
       <c r="E27">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="G27">
-        <v>1519</v>
+        <v>1754</v>
       </c>
       <c r="H27" t="s">
         <v>50</v>
@@ -1449,7 +1440,7 @@
         <v>45</v>
       </c>
       <c r="J27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L27" t="s">
         <v>58</v>
@@ -1469,10 +1460,10 @@
         <v>18</v>
       </c>
       <c r="E28">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="G28">
-        <v>1620</v>
+        <v>1519</v>
       </c>
       <c r="H28" t="s">
         <v>50</v>
@@ -1481,7 +1472,7 @@
         <v>45</v>
       </c>
       <c r="J28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L28" t="s">
         <v>58</v>
@@ -1501,10 +1492,10 @@
         <v>18</v>
       </c>
       <c r="E29">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="G29">
-        <v>1408</v>
+        <v>1620</v>
       </c>
       <c r="H29" t="s">
         <v>50</v>
@@ -1513,7 +1504,7 @@
         <v>45</v>
       </c>
       <c r="J29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L29" t="s">
         <v>58</v>
@@ -1533,10 +1524,10 @@
         <v>18</v>
       </c>
       <c r="E30">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="G30">
-        <v>1974</v>
+        <v>1408</v>
       </c>
       <c r="H30" t="s">
         <v>50</v>
@@ -1545,7 +1536,7 @@
         <v>45</v>
       </c>
       <c r="J30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L30" t="s">
         <v>58</v>
@@ -1565,10 +1556,10 @@
         <v>18</v>
       </c>
       <c r="E31">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="G31">
-        <v>1947</v>
+        <v>1974</v>
       </c>
       <c r="H31" t="s">
         <v>50</v>
@@ -1577,7 +1568,7 @@
         <v>45</v>
       </c>
       <c r="J31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L31" t="s">
         <v>58</v>
@@ -1597,10 +1588,10 @@
         <v>18</v>
       </c>
       <c r="E32">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="G32">
-        <v>2418</v>
+        <v>1947</v>
       </c>
       <c r="H32" t="s">
         <v>50</v>
@@ -1609,7 +1600,7 @@
         <v>45</v>
       </c>
       <c r="J32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L32" t="s">
         <v>58</v>
@@ -1629,10 +1620,10 @@
         <v>18</v>
       </c>
       <c r="E33">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="G33">
-        <v>2893</v>
+        <v>2418</v>
       </c>
       <c r="H33" t="s">
         <v>50</v>
@@ -1641,7 +1632,7 @@
         <v>45</v>
       </c>
       <c r="J33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L33" t="s">
         <v>58</v>
@@ -1661,10 +1652,10 @@
         <v>18</v>
       </c>
       <c r="E34">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="G34">
-        <v>2433</v>
+        <v>2893</v>
       </c>
       <c r="H34" t="s">
         <v>50</v>
@@ -1673,7 +1664,7 @@
         <v>45</v>
       </c>
       <c r="J34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L34" t="s">
         <v>58</v>
@@ -1693,10 +1684,10 @@
         <v>18</v>
       </c>
       <c r="E35">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="G35">
-        <v>2631</v>
+        <v>2433</v>
       </c>
       <c r="H35" t="s">
         <v>50</v>
@@ -1705,7 +1696,7 @@
         <v>45</v>
       </c>
       <c r="J35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L35" t="s">
         <v>58</v>
@@ -1725,10 +1716,10 @@
         <v>18</v>
       </c>
       <c r="E36">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="G36">
-        <v>2720</v>
+        <v>2631</v>
       </c>
       <c r="H36" t="s">
         <v>50</v>
@@ -1737,7 +1728,7 @@
         <v>45</v>
       </c>
       <c r="J36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L36" t="s">
         <v>58</v>
@@ -1757,10 +1748,10 @@
         <v>18</v>
       </c>
       <c r="E37">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="G37">
-        <v>2104</v>
+        <v>2720</v>
       </c>
       <c r="H37" t="s">
         <v>50</v>
@@ -1769,7 +1760,7 @@
         <v>45</v>
       </c>
       <c r="J37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L37" t="s">
         <v>58</v>
@@ -1789,10 +1780,10 @@
         <v>18</v>
       </c>
       <c r="E38">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="G38">
-        <v>2685</v>
+        <v>2104</v>
       </c>
       <c r="H38" t="s">
         <v>50</v>
@@ -1801,7 +1792,7 @@
         <v>45</v>
       </c>
       <c r="J38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L38" t="s">
         <v>58</v>
@@ -1821,10 +1812,10 @@
         <v>18</v>
       </c>
       <c r="E39">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="G39">
-        <v>2523</v>
+        <v>2685</v>
       </c>
       <c r="H39" t="s">
         <v>50</v>
@@ -1833,7 +1824,7 @@
         <v>45</v>
       </c>
       <c r="J39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L39" t="s">
         <v>58</v>
@@ -1853,10 +1844,10 @@
         <v>18</v>
       </c>
       <c r="E40">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="G40">
-        <v>2494</v>
+        <v>2523</v>
       </c>
       <c r="H40" t="s">
         <v>50</v>
@@ -1865,7 +1856,7 @@
         <v>45</v>
       </c>
       <c r="J40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L40" t="s">
         <v>58</v>
@@ -1885,10 +1876,10 @@
         <v>18</v>
       </c>
       <c r="E41">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="G41">
-        <v>2466</v>
+        <v>2494</v>
       </c>
       <c r="H41" t="s">
         <v>50</v>
@@ -1897,7 +1888,7 @@
         <v>45</v>
       </c>
       <c r="J41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L41" t="s">
         <v>58</v>
@@ -1917,10 +1908,10 @@
         <v>18</v>
       </c>
       <c r="E42">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="G42">
-        <v>2411</v>
+        <v>2466</v>
       </c>
       <c r="H42" t="s">
         <v>50</v>
@@ -1929,7 +1920,7 @@
         <v>45</v>
       </c>
       <c r="J42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L42" t="s">
         <v>58</v>
@@ -1949,10 +1940,10 @@
         <v>18</v>
       </c>
       <c r="E43">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="G43">
-        <v>2132</v>
+        <v>2411</v>
       </c>
       <c r="H43" t="s">
         <v>50</v>
@@ -1961,7 +1952,7 @@
         <v>45</v>
       </c>
       <c r="J43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L43" t="s">
         <v>58</v>
@@ -1981,10 +1972,10 @@
         <v>18</v>
       </c>
       <c r="E44">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="G44">
-        <v>2355</v>
+        <v>2132</v>
       </c>
       <c r="H44" t="s">
         <v>50</v>
@@ -1993,7 +1984,7 @@
         <v>45</v>
       </c>
       <c r="J44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L44" t="s">
         <v>58</v>
@@ -2013,10 +2004,10 @@
         <v>18</v>
       </c>
       <c r="E45">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="G45">
-        <v>2296</v>
+        <v>2355</v>
       </c>
       <c r="H45" t="s">
         <v>50</v>
@@ -2025,7 +2016,7 @@
         <v>45</v>
       </c>
       <c r="J45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L45" t="s">
         <v>58</v>
@@ -2045,10 +2036,10 @@
         <v>18</v>
       </c>
       <c r="E46">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="G46">
-        <v>2922</v>
+        <v>2296</v>
       </c>
       <c r="H46" t="s">
         <v>50</v>
@@ -2057,7 +2048,7 @@
         <v>45</v>
       </c>
       <c r="J46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L46" t="s">
         <v>58</v>
@@ -2077,10 +2068,10 @@
         <v>18</v>
       </c>
       <c r="E47">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="G47">
-        <v>4160</v>
+        <v>2922</v>
       </c>
       <c r="H47" t="s">
         <v>50</v>
@@ -2089,7 +2080,7 @@
         <v>45</v>
       </c>
       <c r="J47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L47" t="s">
         <v>58</v>
@@ -2109,10 +2100,10 @@
         <v>18</v>
       </c>
       <c r="E48">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="G48">
-        <v>3987</v>
+        <v>4160</v>
       </c>
       <c r="H48" t="s">
         <v>50</v>
@@ -2121,7 +2112,7 @@
         <v>45</v>
       </c>
       <c r="J48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L48" t="s">
         <v>58</v>
@@ -2141,10 +2132,10 @@
         <v>18</v>
       </c>
       <c r="E49">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="G49">
-        <v>4133</v>
+        <v>3987</v>
       </c>
       <c r="H49" t="s">
         <v>50</v>
@@ -2153,7 +2144,7 @@
         <v>45</v>
       </c>
       <c r="J49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L49" t="s">
         <v>58</v>
@@ -2167,25 +2158,28 @@
         <v>19</v>
       </c>
       <c r="C50" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D50" t="s">
         <v>18</v>
       </c>
       <c r="E50">
-        <v>1990</v>
+        <v>2019</v>
       </c>
       <c r="G50">
-        <v>1770</v>
+        <v>4133</v>
       </c>
       <c r="H50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I50" t="s">
         <v>45</v>
       </c>
       <c r="J50" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+      <c r="L50" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
@@ -2202,7 +2196,7 @@
         <v>18</v>
       </c>
       <c r="E51">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="G51">
         <v>1770</v>
@@ -2213,6 +2207,9 @@
       <c r="I51" t="s">
         <v>45</v>
       </c>
+      <c r="J51" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
@@ -2228,7 +2225,7 @@
         <v>18</v>
       </c>
       <c r="E52">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="G52">
         <v>1770</v>
@@ -2254,7 +2251,7 @@
         <v>18</v>
       </c>
       <c r="E53">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="G53">
         <v>1770</v>
@@ -2280,7 +2277,7 @@
         <v>18</v>
       </c>
       <c r="E54">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="G54">
         <v>1770</v>
@@ -2306,7 +2303,7 @@
         <v>18</v>
       </c>
       <c r="E55">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="G55">
         <v>1770</v>
@@ -2332,7 +2329,7 @@
         <v>18</v>
       </c>
       <c r="E56">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="G56">
         <v>1770</v>
@@ -2358,7 +2355,7 @@
         <v>18</v>
       </c>
       <c r="E57">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="G57">
         <v>1770</v>
@@ -2384,7 +2381,7 @@
         <v>18</v>
       </c>
       <c r="E58">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="G58">
         <v>1770</v>
@@ -2410,7 +2407,7 @@
         <v>18</v>
       </c>
       <c r="E59">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="G59">
         <v>1770</v>
@@ -2436,19 +2433,16 @@
         <v>18</v>
       </c>
       <c r="E60">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="G60">
-        <v>1760</v>
+        <v>1770</v>
       </c>
       <c r="H60" t="s">
         <v>51</v>
       </c>
       <c r="I60" t="s">
         <v>45</v>
-      </c>
-      <c r="J60" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
@@ -2465,7 +2459,7 @@
         <v>18</v>
       </c>
       <c r="E61">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="G61">
         <v>1760</v>
@@ -2476,6 +2470,9 @@
       <c r="I61" t="s">
         <v>45</v>
       </c>
+      <c r="J61" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
@@ -2491,7 +2488,7 @@
         <v>18</v>
       </c>
       <c r="E62">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="G62">
         <v>1760</v>
@@ -2517,7 +2514,7 @@
         <v>18</v>
       </c>
       <c r="E63">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="G63">
         <v>1760</v>
@@ -2543,7 +2540,7 @@
         <v>18</v>
       </c>
       <c r="E64">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="G64">
         <v>1760</v>
@@ -2555,7 +2552,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>16</v>
       </c>
@@ -2569,10 +2566,10 @@
         <v>18</v>
       </c>
       <c r="E65">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="G65">
-        <v>1700</v>
+        <v>1760</v>
       </c>
       <c r="H65" t="s">
         <v>51</v>
@@ -2580,11 +2577,8 @@
       <c r="I65" t="s">
         <v>45</v>
       </c>
-      <c r="J65" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>16</v>
       </c>
@@ -2598,7 +2592,7 @@
         <v>18</v>
       </c>
       <c r="E66">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="G66">
         <v>1700</v>
@@ -2609,8 +2603,11 @@
       <c r="I66" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J66" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>16</v>
       </c>
@@ -2624,7 +2621,7 @@
         <v>18</v>
       </c>
       <c r="E67">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="G67">
         <v>1700</v>
@@ -2636,7 +2633,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>16</v>
       </c>
@@ -2650,7 +2647,7 @@
         <v>18</v>
       </c>
       <c r="E68">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="G68">
         <v>1700</v>
@@ -2662,7 +2659,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>16</v>
       </c>
@@ -2676,7 +2673,7 @@
         <v>18</v>
       </c>
       <c r="E69">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="G69">
         <v>1700</v>
@@ -2688,7 +2685,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>16</v>
       </c>
@@ -2702,10 +2699,10 @@
         <v>18</v>
       </c>
       <c r="E70">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="G70">
-        <v>1840</v>
+        <v>1700</v>
       </c>
       <c r="H70" t="s">
         <v>51</v>
@@ -2713,11 +2710,8 @@
       <c r="I70" t="s">
         <v>45</v>
       </c>
-      <c r="J70" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>16</v>
       </c>
@@ -2731,7 +2725,7 @@
         <v>18</v>
       </c>
       <c r="E71">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="G71">
         <v>1840</v>
@@ -2746,7 +2740,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>16</v>
       </c>
@@ -2760,7 +2754,7 @@
         <v>18</v>
       </c>
       <c r="E72">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="G72">
         <v>1840</v>
@@ -2775,7 +2769,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>16</v>
       </c>
@@ -2789,7 +2783,7 @@
         <v>18</v>
       </c>
       <c r="E73">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="G73">
         <v>1840</v>
@@ -2804,7 +2798,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>16</v>
       </c>
@@ -2818,7 +2812,7 @@
         <v>18</v>
       </c>
       <c r="E74">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="G74">
         <v>1840</v>
@@ -2833,7 +2827,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>16</v>
       </c>
@@ -2847,7 +2841,7 @@
         <v>18</v>
       </c>
       <c r="E75">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="G75">
         <v>1840</v>
@@ -2858,8 +2852,11 @@
       <c r="I75" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J75" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>16</v>
       </c>
@@ -2873,7 +2870,7 @@
         <v>18</v>
       </c>
       <c r="E76">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="G76">
         <v>1840</v>
@@ -2885,7 +2882,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>16</v>
       </c>
@@ -2899,7 +2896,7 @@
         <v>18</v>
       </c>
       <c r="E77">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="G77">
         <v>1840</v>
@@ -2911,7 +2908,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>16</v>
       </c>
@@ -2925,7 +2922,7 @@
         <v>18</v>
       </c>
       <c r="E78">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="G78">
         <v>1840</v>
@@ -2937,7 +2934,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>16</v>
       </c>
@@ -2951,7 +2948,7 @@
         <v>18</v>
       </c>
       <c r="E79">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="G79">
         <v>1840</v>
@@ -2963,7 +2960,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>16</v>
       </c>
@@ -2971,25 +2968,22 @@
         <v>19</v>
       </c>
       <c r="C80" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D80" t="s">
         <v>18</v>
       </c>
       <c r="E80">
-        <v>1990</v>
+        <v>2019</v>
       </c>
       <c r="G80">
-        <v>0</v>
+        <v>1840</v>
       </c>
       <c r="H80" t="s">
         <v>51</v>
       </c>
       <c r="I80" t="s">
         <v>45</v>
-      </c>
-      <c r="L80" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.2">
@@ -3006,7 +3000,7 @@
         <v>18</v>
       </c>
       <c r="E81">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -3035,7 +3029,7 @@
         <v>18</v>
       </c>
       <c r="E82">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -3064,7 +3058,7 @@
         <v>18</v>
       </c>
       <c r="E83">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -3093,7 +3087,7 @@
         <v>18</v>
       </c>
       <c r="E84">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -3122,7 +3116,7 @@
         <v>18</v>
       </c>
       <c r="E85">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -3151,7 +3145,7 @@
         <v>18</v>
       </c>
       <c r="E86">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="G86">
         <v>0</v>
@@ -3180,7 +3174,7 @@
         <v>18</v>
       </c>
       <c r="E87">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -3209,7 +3203,7 @@
         <v>18</v>
       </c>
       <c r="E88">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="G88">
         <v>0</v>
@@ -3238,7 +3232,7 @@
         <v>18</v>
       </c>
       <c r="E89">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="G89">
         <v>0</v>
@@ -3267,7 +3261,7 @@
         <v>18</v>
       </c>
       <c r="E90">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -3296,7 +3290,7 @@
         <v>18</v>
       </c>
       <c r="E91">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -3325,7 +3319,7 @@
         <v>18</v>
       </c>
       <c r="E92">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="G92">
         <v>0</v>
@@ -3354,7 +3348,7 @@
         <v>18</v>
       </c>
       <c r="E93">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -3383,7 +3377,7 @@
         <v>18</v>
       </c>
       <c r="E94">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -3412,7 +3406,7 @@
         <v>18</v>
       </c>
       <c r="E95">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -3441,7 +3435,7 @@
         <v>18</v>
       </c>
       <c r="E96">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -3470,7 +3464,7 @@
         <v>18</v>
       </c>
       <c r="E97">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -3499,7 +3493,7 @@
         <v>18</v>
       </c>
       <c r="E98">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -3528,7 +3522,7 @@
         <v>18</v>
       </c>
       <c r="E99">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -3557,10 +3551,10 @@
         <v>18</v>
       </c>
       <c r="E100">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="G100">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="H100" t="s">
         <v>51</v>
@@ -3586,10 +3580,10 @@
         <v>18</v>
       </c>
       <c r="E101">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="G101">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="H101" t="s">
         <v>51</v>
@@ -3615,7 +3609,7 @@
         <v>18</v>
       </c>
       <c r="E102">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="G102">
         <v>0</v>
@@ -3644,7 +3638,7 @@
         <v>18</v>
       </c>
       <c r="E103">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -3673,7 +3667,7 @@
         <v>18</v>
       </c>
       <c r="E104">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -3702,7 +3696,7 @@
         <v>18</v>
       </c>
       <c r="E105">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="G105">
         <v>0</v>
@@ -3731,7 +3725,7 @@
         <v>18</v>
       </c>
       <c r="E106">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -3760,7 +3754,7 @@
         <v>18</v>
       </c>
       <c r="E107">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="G107">
         <v>0</v>
@@ -3789,7 +3783,7 @@
         <v>18</v>
       </c>
       <c r="E108">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="G108">
         <v>0</v>
@@ -3818,7 +3812,7 @@
         <v>18</v>
       </c>
       <c r="E109">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="G109">
         <v>0</v>
@@ -3841,13 +3835,13 @@
         <v>19</v>
       </c>
       <c r="C110" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D110" t="s">
         <v>18</v>
       </c>
       <c r="E110">
-        <v>1990</v>
+        <v>2019</v>
       </c>
       <c r="G110">
         <v>0</v>
@@ -3876,7 +3870,7 @@
         <v>18</v>
       </c>
       <c r="E111">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="G111">
         <v>0</v>
@@ -3905,7 +3899,7 @@
         <v>18</v>
       </c>
       <c r="E112">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="G112">
         <v>0</v>
@@ -3934,7 +3928,7 @@
         <v>18</v>
       </c>
       <c r="E113">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="G113">
         <v>0</v>
@@ -3963,7 +3957,7 @@
         <v>18</v>
       </c>
       <c r="E114">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="G114">
         <v>0</v>
@@ -3992,7 +3986,7 @@
         <v>18</v>
       </c>
       <c r="E115">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="G115">
         <v>0</v>
@@ -4021,7 +4015,7 @@
         <v>18</v>
       </c>
       <c r="E116">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="G116">
         <v>0</v>
@@ -4050,7 +4044,7 @@
         <v>18</v>
       </c>
       <c r="E117">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -4079,7 +4073,7 @@
         <v>18</v>
       </c>
       <c r="E118">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="G118">
         <v>0</v>
@@ -4108,7 +4102,7 @@
         <v>18</v>
       </c>
       <c r="E119">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="G119">
         <v>0</v>
@@ -4137,10 +4131,10 @@
         <v>18</v>
       </c>
       <c r="E120">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="G120">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H120" t="s">
         <v>51</v>
@@ -4166,10 +4160,10 @@
         <v>18</v>
       </c>
       <c r="E121">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="G121">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H121" t="s">
         <v>51</v>
@@ -4195,7 +4189,7 @@
         <v>18</v>
       </c>
       <c r="E122">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="G122">
         <v>0</v>
@@ -4224,7 +4218,7 @@
         <v>18</v>
       </c>
       <c r="E123">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="G123">
         <v>0</v>
@@ -4253,7 +4247,7 @@
         <v>18</v>
       </c>
       <c r="E124">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="G124">
         <v>0</v>
@@ -4282,10 +4276,10 @@
         <v>18</v>
       </c>
       <c r="E125">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="G125">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="H125" t="s">
         <v>51</v>
@@ -4311,10 +4305,10 @@
         <v>18</v>
       </c>
       <c r="E126">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="G126">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="H126" t="s">
         <v>51</v>
@@ -4340,7 +4334,7 @@
         <v>18</v>
       </c>
       <c r="E127">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="G127">
         <v>0</v>
@@ -4369,7 +4363,7 @@
         <v>18</v>
       </c>
       <c r="E128">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="G128">
         <v>0</v>
@@ -4398,7 +4392,7 @@
         <v>18</v>
       </c>
       <c r="E129">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="G129">
         <v>0</v>
@@ -4427,7 +4421,7 @@
         <v>18</v>
       </c>
       <c r="E130">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="G130">
         <v>0</v>
@@ -4456,7 +4450,7 @@
         <v>18</v>
       </c>
       <c r="E131">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="G131">
         <v>0</v>
@@ -4485,7 +4479,7 @@
         <v>18</v>
       </c>
       <c r="E132">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="G132">
         <v>0</v>
@@ -4514,7 +4508,7 @@
         <v>18</v>
       </c>
       <c r="E133">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="G133">
         <v>0</v>
@@ -4543,7 +4537,7 @@
         <v>18</v>
       </c>
       <c r="E134">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="G134">
         <v>0</v>
@@ -4572,7 +4566,7 @@
         <v>18</v>
       </c>
       <c r="E135">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="G135">
         <v>0</v>
@@ -4601,7 +4595,7 @@
         <v>18</v>
       </c>
       <c r="E136">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="G136">
         <v>0</v>
@@ -4630,7 +4624,7 @@
         <v>18</v>
       </c>
       <c r="E137">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="G137">
         <v>0</v>
@@ -4659,7 +4653,7 @@
         <v>18</v>
       </c>
       <c r="E138">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="G138">
         <v>0</v>
@@ -4688,7 +4682,7 @@
         <v>18</v>
       </c>
       <c r="E139">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="G139">
         <v>0</v>
@@ -4711,13 +4705,25 @@
         <v>19</v>
       </c>
       <c r="C140" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D140" t="s">
         <v>18</v>
       </c>
       <c r="E140">
-        <v>1990</v>
+        <v>2019</v>
+      </c>
+      <c r="G140">
+        <v>0</v>
+      </c>
+      <c r="H140" t="s">
+        <v>51</v>
+      </c>
+      <c r="I140" t="s">
+        <v>45</v>
+      </c>
+      <c r="L140" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.2">
@@ -4734,7 +4740,7 @@
         <v>18</v>
       </c>
       <c r="E141">
-        <v>1991</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.2">
@@ -4751,7 +4757,7 @@
         <v>18</v>
       </c>
       <c r="E142">
-        <v>1992</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.2">
@@ -4768,7 +4774,7 @@
         <v>18</v>
       </c>
       <c r="E143">
-        <v>1993</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.2">
@@ -4785,7 +4791,7 @@
         <v>18</v>
       </c>
       <c r="E144">
-        <v>1994</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
@@ -4802,7 +4808,7 @@
         <v>18</v>
       </c>
       <c r="E145">
-        <v>1995</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
@@ -4819,7 +4825,7 @@
         <v>18</v>
       </c>
       <c r="E146">
-        <v>1996</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
@@ -4836,7 +4842,7 @@
         <v>18</v>
       </c>
       <c r="E147">
-        <v>1997</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
@@ -4853,7 +4859,7 @@
         <v>18</v>
       </c>
       <c r="E148">
-        <v>1998</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
@@ -4870,7 +4876,7 @@
         <v>18</v>
       </c>
       <c r="E149">
-        <v>1999</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
@@ -4887,7 +4893,7 @@
         <v>18</v>
       </c>
       <c r="E150">
-        <v>2000</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
@@ -4904,7 +4910,7 @@
         <v>18</v>
       </c>
       <c r="E151">
-        <v>2001</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
@@ -4921,7 +4927,7 @@
         <v>18</v>
       </c>
       <c r="E152">
-        <v>2002</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
@@ -4938,7 +4944,7 @@
         <v>18</v>
       </c>
       <c r="E153">
-        <v>2003</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
@@ -4955,7 +4961,7 @@
         <v>18</v>
       </c>
       <c r="E154">
-        <v>2004</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
@@ -4972,7 +4978,7 @@
         <v>18</v>
       </c>
       <c r="E155">
-        <v>2005</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
@@ -4989,7 +4995,7 @@
         <v>18</v>
       </c>
       <c r="E156">
-        <v>2006</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
@@ -5006,7 +5012,7 @@
         <v>18</v>
       </c>
       <c r="E157">
-        <v>2007</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
@@ -5023,7 +5029,7 @@
         <v>18</v>
       </c>
       <c r="E158">
-        <v>2008</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
@@ -5040,7 +5046,7 @@
         <v>18</v>
       </c>
       <c r="E159">
-        <v>2009</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
@@ -5057,7 +5063,7 @@
         <v>18</v>
       </c>
       <c r="E160">
-        <v>2010</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.2">
@@ -5074,22 +5080,7 @@
         <v>18</v>
       </c>
       <c r="E161">
-        <v>2011</v>
-      </c>
-      <c r="G161">
-        <v>33.53</v>
-      </c>
-      <c r="H161" t="s">
-        <v>90</v>
-      </c>
-      <c r="I161" t="s">
-        <v>45</v>
-      </c>
-      <c r="J161" t="s">
-        <v>91</v>
-      </c>
-      <c r="L161" t="s">
-        <v>92</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="162" spans="1:12" x14ac:dyDescent="0.2">
@@ -5106,7 +5097,22 @@
         <v>18</v>
       </c>
       <c r="E162">
-        <v>2012</v>
+        <v>2011</v>
+      </c>
+      <c r="G162">
+        <v>33.53</v>
+      </c>
+      <c r="H162" t="s">
+        <v>90</v>
+      </c>
+      <c r="I162" t="s">
+        <v>45</v>
+      </c>
+      <c r="J162" t="s">
+        <v>91</v>
+      </c>
+      <c r="L162" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="163" spans="1:12" x14ac:dyDescent="0.2">
@@ -5123,7 +5129,7 @@
         <v>18</v>
       </c>
       <c r="E163">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="164" spans="1:12" x14ac:dyDescent="0.2">
@@ -5140,7 +5146,7 @@
         <v>18</v>
       </c>
       <c r="E164">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="165" spans="1:12" x14ac:dyDescent="0.2">
@@ -5157,7 +5163,7 @@
         <v>18</v>
       </c>
       <c r="E165">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="166" spans="1:12" x14ac:dyDescent="0.2">
@@ -5174,7 +5180,7 @@
         <v>18</v>
       </c>
       <c r="E166">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="167" spans="1:12" x14ac:dyDescent="0.2">
@@ -5191,7 +5197,7 @@
         <v>18</v>
       </c>
       <c r="E167">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="168" spans="1:12" x14ac:dyDescent="0.2">
@@ -5208,7 +5214,7 @@
         <v>18</v>
       </c>
       <c r="E168">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="169" spans="1:12" x14ac:dyDescent="0.2">
@@ -5225,7 +5231,7 @@
         <v>18</v>
       </c>
       <c r="E169">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="170" spans="1:12" x14ac:dyDescent="0.2">
@@ -5236,13 +5242,13 @@
         <v>19</v>
       </c>
       <c r="C170" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D170" t="s">
         <v>18</v>
       </c>
       <c r="E170">
-        <v>1990</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="171" spans="1:12" x14ac:dyDescent="0.2">
@@ -5259,7 +5265,7 @@
         <v>18</v>
       </c>
       <c r="E171">
-        <v>1991</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="172" spans="1:12" x14ac:dyDescent="0.2">
@@ -5276,7 +5282,7 @@
         <v>18</v>
       </c>
       <c r="E172">
-        <v>1992</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="173" spans="1:12" x14ac:dyDescent="0.2">
@@ -5293,7 +5299,7 @@
         <v>18</v>
       </c>
       <c r="E173">
-        <v>1993</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="174" spans="1:12" x14ac:dyDescent="0.2">
@@ -5310,7 +5316,7 @@
         <v>18</v>
       </c>
       <c r="E174">
-        <v>1994</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="175" spans="1:12" x14ac:dyDescent="0.2">
@@ -5327,7 +5333,7 @@
         <v>18</v>
       </c>
       <c r="E175">
-        <v>1995</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.2">
@@ -5344,7 +5350,7 @@
         <v>18</v>
       </c>
       <c r="E176">
-        <v>1996</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="177" spans="1:12" x14ac:dyDescent="0.2">
@@ -5361,7 +5367,7 @@
         <v>18</v>
       </c>
       <c r="E177">
-        <v>1997</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="178" spans="1:12" x14ac:dyDescent="0.2">
@@ -5378,7 +5384,7 @@
         <v>18</v>
       </c>
       <c r="E178">
-        <v>1998</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="179" spans="1:12" x14ac:dyDescent="0.2">
@@ -5395,7 +5401,7 @@
         <v>18</v>
       </c>
       <c r="E179">
-        <v>1999</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="180" spans="1:12" x14ac:dyDescent="0.2">
@@ -5412,7 +5418,7 @@
         <v>18</v>
       </c>
       <c r="E180">
-        <v>2000</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="181" spans="1:12" x14ac:dyDescent="0.2">
@@ -5429,7 +5435,7 @@
         <v>18</v>
       </c>
       <c r="E181">
-        <v>2001</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="182" spans="1:12" x14ac:dyDescent="0.2">
@@ -5446,7 +5452,7 @@
         <v>18</v>
       </c>
       <c r="E182">
-        <v>2002</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="183" spans="1:12" x14ac:dyDescent="0.2">
@@ -5463,7 +5469,7 @@
         <v>18</v>
       </c>
       <c r="E183">
-        <v>2003</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="184" spans="1:12" x14ac:dyDescent="0.2">
@@ -5480,7 +5486,7 @@
         <v>18</v>
       </c>
       <c r="E184">
-        <v>2004</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="185" spans="1:12" x14ac:dyDescent="0.2">
@@ -5497,7 +5503,7 @@
         <v>18</v>
       </c>
       <c r="E185">
-        <v>2005</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="186" spans="1:12" x14ac:dyDescent="0.2">
@@ -5514,7 +5520,7 @@
         <v>18</v>
       </c>
       <c r="E186">
-        <v>2006</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="187" spans="1:12" x14ac:dyDescent="0.2">
@@ -5531,7 +5537,7 @@
         <v>18</v>
       </c>
       <c r="E187">
-        <v>2007</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="188" spans="1:12" x14ac:dyDescent="0.2">
@@ -5548,7 +5554,7 @@
         <v>18</v>
       </c>
       <c r="E188">
-        <v>2008</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="189" spans="1:12" x14ac:dyDescent="0.2">
@@ -5565,7 +5571,7 @@
         <v>18</v>
       </c>
       <c r="E189">
-        <v>2009</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="190" spans="1:12" x14ac:dyDescent="0.2">
@@ -5582,7 +5588,7 @@
         <v>18</v>
       </c>
       <c r="E190">
-        <v>2010</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="191" spans="1:12" x14ac:dyDescent="0.2">
@@ -5599,22 +5605,7 @@
         <v>18</v>
       </c>
       <c r="E191">
-        <v>2011</v>
-      </c>
-      <c r="G191">
-        <v>1869</v>
-      </c>
-      <c r="H191" t="s">
-        <v>90</v>
-      </c>
-      <c r="I191" t="s">
-        <v>45</v>
-      </c>
-      <c r="J191" t="s">
-        <v>91</v>
-      </c>
-      <c r="L191" t="s">
-        <v>92</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="192" spans="1:12" x14ac:dyDescent="0.2">
@@ -5631,7 +5622,22 @@
         <v>18</v>
       </c>
       <c r="E192">
-        <v>2012</v>
+        <v>2011</v>
+      </c>
+      <c r="G192">
+        <v>1869</v>
+      </c>
+      <c r="H192" t="s">
+        <v>90</v>
+      </c>
+      <c r="I192" t="s">
+        <v>45</v>
+      </c>
+      <c r="J192" t="s">
+        <v>91</v>
+      </c>
+      <c r="L192" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
@@ -5648,7 +5654,7 @@
         <v>18</v>
       </c>
       <c r="E193">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
@@ -5665,7 +5671,7 @@
         <v>18</v>
       </c>
       <c r="E194">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
@@ -5682,7 +5688,7 @@
         <v>18</v>
       </c>
       <c r="E195">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
@@ -5699,7 +5705,7 @@
         <v>18</v>
       </c>
       <c r="E196">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
@@ -5716,7 +5722,7 @@
         <v>18</v>
       </c>
       <c r="E197">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
@@ -5733,7 +5739,7 @@
         <v>18</v>
       </c>
       <c r="E198">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
@@ -5750,7 +5756,7 @@
         <v>18</v>
       </c>
       <c r="E199">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
@@ -5761,13 +5767,13 @@
         <v>19</v>
       </c>
       <c r="C200" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D200" t="s">
         <v>18</v>
       </c>
       <c r="E200">
-        <v>1990</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
@@ -5784,7 +5790,7 @@
         <v>18</v>
       </c>
       <c r="E201">
-        <v>1991</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
@@ -5801,7 +5807,7 @@
         <v>18</v>
       </c>
       <c r="E202">
-        <v>1992</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
@@ -5818,7 +5824,7 @@
         <v>18</v>
       </c>
       <c r="E203">
-        <v>1993</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
@@ -5835,7 +5841,7 @@
         <v>18</v>
       </c>
       <c r="E204">
-        <v>1994</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
@@ -5852,7 +5858,7 @@
         <v>18</v>
       </c>
       <c r="E205">
-        <v>1995</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
@@ -5869,7 +5875,7 @@
         <v>18</v>
       </c>
       <c r="E206">
-        <v>1996</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
@@ -5886,7 +5892,7 @@
         <v>18</v>
       </c>
       <c r="E207">
-        <v>1997</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
@@ -5903,7 +5909,7 @@
         <v>18</v>
       </c>
       <c r="E208">
-        <v>1998</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="209" spans="1:12" x14ac:dyDescent="0.2">
@@ -5920,7 +5926,7 @@
         <v>18</v>
       </c>
       <c r="E209">
-        <v>1999</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="210" spans="1:12" x14ac:dyDescent="0.2">
@@ -5937,7 +5943,7 @@
         <v>18</v>
       </c>
       <c r="E210">
-        <v>2000</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="211" spans="1:12" x14ac:dyDescent="0.2">
@@ -5954,7 +5960,7 @@
         <v>18</v>
       </c>
       <c r="E211">
-        <v>2001</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="212" spans="1:12" x14ac:dyDescent="0.2">
@@ -5971,7 +5977,7 @@
         <v>18</v>
       </c>
       <c r="E212">
-        <v>2002</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="213" spans="1:12" x14ac:dyDescent="0.2">
@@ -5988,7 +5994,7 @@
         <v>18</v>
       </c>
       <c r="E213">
-        <v>2003</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="214" spans="1:12" x14ac:dyDescent="0.2">
@@ -6005,7 +6011,7 @@
         <v>18</v>
       </c>
       <c r="E214">
-        <v>2004</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="215" spans="1:12" x14ac:dyDescent="0.2">
@@ -6022,7 +6028,7 @@
         <v>18</v>
       </c>
       <c r="E215">
-        <v>2005</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="216" spans="1:12" x14ac:dyDescent="0.2">
@@ -6039,7 +6045,7 @@
         <v>18</v>
       </c>
       <c r="E216">
-        <v>2006</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="217" spans="1:12" x14ac:dyDescent="0.2">
@@ -6056,7 +6062,7 @@
         <v>18</v>
       </c>
       <c r="E217">
-        <v>2007</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="218" spans="1:12" x14ac:dyDescent="0.2">
@@ -6073,7 +6079,7 @@
         <v>18</v>
       </c>
       <c r="E218">
-        <v>2008</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="219" spans="1:12" x14ac:dyDescent="0.2">
@@ -6090,7 +6096,7 @@
         <v>18</v>
       </c>
       <c r="E219">
-        <v>2009</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="220" spans="1:12" x14ac:dyDescent="0.2">
@@ -6107,7 +6113,7 @@
         <v>18</v>
       </c>
       <c r="E220">
-        <v>2010</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="221" spans="1:12" x14ac:dyDescent="0.2">
@@ -6124,22 +6130,7 @@
         <v>18</v>
       </c>
       <c r="E221">
-        <v>2011</v>
-      </c>
-      <c r="G221">
-        <v>0</v>
-      </c>
-      <c r="H221" t="s">
-        <v>93</v>
-      </c>
-      <c r="I221" t="s">
-        <v>45</v>
-      </c>
-      <c r="J221" t="s">
-        <v>91</v>
-      </c>
-      <c r="L221" t="s">
-        <v>92</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="222" spans="1:12" x14ac:dyDescent="0.2">
@@ -6156,7 +6147,22 @@
         <v>18</v>
       </c>
       <c r="E222">
-        <v>2012</v>
+        <v>2011</v>
+      </c>
+      <c r="G222">
+        <v>0</v>
+      </c>
+      <c r="H222" t="s">
+        <v>93</v>
+      </c>
+      <c r="I222" t="s">
+        <v>45</v>
+      </c>
+      <c r="J222" t="s">
+        <v>91</v>
+      </c>
+      <c r="L222" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="223" spans="1:12" x14ac:dyDescent="0.2">
@@ -6173,7 +6179,7 @@
         <v>18</v>
       </c>
       <c r="E223">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="224" spans="1:12" x14ac:dyDescent="0.2">
@@ -6190,7 +6196,7 @@
         <v>18</v>
       </c>
       <c r="E224">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="225" spans="1:12" x14ac:dyDescent="0.2">
@@ -6207,7 +6213,7 @@
         <v>18</v>
       </c>
       <c r="E225">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="226" spans="1:12" x14ac:dyDescent="0.2">
@@ -6224,7 +6230,7 @@
         <v>18</v>
       </c>
       <c r="E226">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="227" spans="1:12" x14ac:dyDescent="0.2">
@@ -6241,7 +6247,7 @@
         <v>18</v>
       </c>
       <c r="E227">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="228" spans="1:12" x14ac:dyDescent="0.2">
@@ -6258,7 +6264,7 @@
         <v>18</v>
       </c>
       <c r="E228">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="229" spans="1:12" x14ac:dyDescent="0.2">
@@ -6275,7 +6281,7 @@
         <v>18</v>
       </c>
       <c r="E229">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="230" spans="1:12" x14ac:dyDescent="0.2">
@@ -6286,25 +6292,13 @@
         <v>19</v>
       </c>
       <c r="C230" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D230" t="s">
         <v>18</v>
       </c>
       <c r="E230">
-        <v>1990</v>
-      </c>
-      <c r="G230">
-        <v>0</v>
-      </c>
-      <c r="H230" t="s">
-        <v>51</v>
-      </c>
-      <c r="I230" t="s">
-        <v>45</v>
-      </c>
-      <c r="L230" t="s">
-        <v>94</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="231" spans="1:12" x14ac:dyDescent="0.2">
@@ -6321,7 +6315,7 @@
         <v>18</v>
       </c>
       <c r="E231">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="G231">
         <v>0</v>
@@ -6350,7 +6344,7 @@
         <v>18</v>
       </c>
       <c r="E232">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="G232">
         <v>0</v>
@@ -6379,7 +6373,7 @@
         <v>18</v>
       </c>
       <c r="E233">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="G233">
         <v>0</v>
@@ -6408,7 +6402,7 @@
         <v>18</v>
       </c>
       <c r="E234">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="G234">
         <v>0</v>
@@ -6437,7 +6431,7 @@
         <v>18</v>
       </c>
       <c r="E235">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="G235">
         <v>0</v>
@@ -6466,7 +6460,7 @@
         <v>18</v>
       </c>
       <c r="E236">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="G236">
         <v>0</v>
@@ -6495,7 +6489,7 @@
         <v>18</v>
       </c>
       <c r="E237">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="G237">
         <v>0</v>
@@ -6524,7 +6518,7 @@
         <v>18</v>
       </c>
       <c r="E238">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="G238">
         <v>0</v>
@@ -6553,7 +6547,7 @@
         <v>18</v>
       </c>
       <c r="E239">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="G239">
         <v>0</v>
@@ -6582,10 +6576,10 @@
         <v>18</v>
       </c>
       <c r="E240">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="G240">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H240" t="s">
         <v>51</v>
@@ -6611,10 +6605,10 @@
         <v>18</v>
       </c>
       <c r="E241">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="G241">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H241" t="s">
         <v>51</v>
@@ -6640,7 +6634,7 @@
         <v>18</v>
       </c>
       <c r="E242">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="G242">
         <v>0</v>
@@ -6669,7 +6663,7 @@
         <v>18</v>
       </c>
       <c r="E243">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="G243">
         <v>0</v>
@@ -6698,7 +6692,7 @@
         <v>18</v>
       </c>
       <c r="E244">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="G244">
         <v>0</v>
@@ -6727,10 +6721,10 @@
         <v>18</v>
       </c>
       <c r="E245">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="G245">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="H245" t="s">
         <v>51</v>
@@ -6756,10 +6750,10 @@
         <v>18</v>
       </c>
       <c r="E246">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="G246">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="H246" t="s">
         <v>51</v>
@@ -6785,7 +6779,7 @@
         <v>18</v>
       </c>
       <c r="E247">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="G247">
         <v>0</v>
@@ -6814,7 +6808,7 @@
         <v>18</v>
       </c>
       <c r="E248">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="G248">
         <v>0</v>
@@ -6843,7 +6837,7 @@
         <v>18</v>
       </c>
       <c r="E249">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="G249">
         <v>0</v>
@@ -6872,7 +6866,7 @@
         <v>18</v>
       </c>
       <c r="E250">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="G250">
         <v>0</v>
@@ -6901,7 +6895,7 @@
         <v>18</v>
       </c>
       <c r="E251">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="G251">
         <v>0</v>
@@ -6930,7 +6924,7 @@
         <v>18</v>
       </c>
       <c r="E252">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="G252">
         <v>0</v>
@@ -6959,7 +6953,7 @@
         <v>18</v>
       </c>
       <c r="E253">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="G253">
         <v>0</v>
@@ -6988,7 +6982,7 @@
         <v>18</v>
       </c>
       <c r="E254">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="G254">
         <v>0</v>
@@ -7017,7 +7011,7 @@
         <v>18</v>
       </c>
       <c r="E255">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="G255">
         <v>0</v>
@@ -7046,7 +7040,7 @@
         <v>18</v>
       </c>
       <c r="E256">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="G256">
         <v>0</v>
@@ -7075,7 +7069,7 @@
         <v>18</v>
       </c>
       <c r="E257">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="G257">
         <v>0</v>
@@ -7104,7 +7098,7 @@
         <v>18</v>
       </c>
       <c r="E258">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="G258">
         <v>0</v>
@@ -7133,7 +7127,7 @@
         <v>18</v>
       </c>
       <c r="E259">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="G259">
         <v>0</v>
@@ -7156,22 +7150,25 @@
         <v>19</v>
       </c>
       <c r="C260" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D260" t="s">
         <v>18</v>
       </c>
       <c r="E260">
-        <v>1990</v>
+        <v>2019</v>
       </c>
       <c r="G260">
-        <v>0.4</v>
+        <v>0</v>
+      </c>
+      <c r="H260" t="s">
+        <v>51</v>
       </c>
       <c r="I260" t="s">
         <v>45</v>
       </c>
-      <c r="J260" t="s">
-        <v>46</v>
+      <c r="L260" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="261" spans="1:12" x14ac:dyDescent="0.2">
@@ -7188,7 +7185,7 @@
         <v>18</v>
       </c>
       <c r="E261">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="G261">
         <v>0.4</v>
@@ -7214,7 +7211,7 @@
         <v>18</v>
       </c>
       <c r="E262">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="G262">
         <v>0.4</v>
@@ -7240,7 +7237,7 @@
         <v>18</v>
       </c>
       <c r="E263">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="G263">
         <v>0.4</v>
@@ -7266,7 +7263,7 @@
         <v>18</v>
       </c>
       <c r="E264">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="G264">
         <v>0.4</v>
@@ -7292,7 +7289,7 @@
         <v>18</v>
       </c>
       <c r="E265">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="G265">
         <v>0.4</v>
@@ -7318,7 +7315,7 @@
         <v>18</v>
       </c>
       <c r="E266">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="G266">
         <v>0.4</v>
@@ -7344,7 +7341,7 @@
         <v>18</v>
       </c>
       <c r="E267">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="G267">
         <v>0.4</v>
@@ -7370,7 +7367,7 @@
         <v>18</v>
       </c>
       <c r="E268">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="G268">
         <v>0.4</v>
@@ -7396,7 +7393,7 @@
         <v>18</v>
       </c>
       <c r="E269">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="G269">
         <v>0.4</v>
@@ -7422,7 +7419,7 @@
         <v>18</v>
       </c>
       <c r="E270">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="G270">
         <v>0.4</v>
@@ -7448,7 +7445,7 @@
         <v>18</v>
       </c>
       <c r="E271">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="G271">
         <v>0.4</v>
@@ -7474,7 +7471,7 @@
         <v>18</v>
       </c>
       <c r="E272">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="G272">
         <v>0.4</v>
@@ -7500,7 +7497,7 @@
         <v>18</v>
       </c>
       <c r="E273">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="G273">
         <v>0.4</v>
@@ -7526,7 +7523,7 @@
         <v>18</v>
       </c>
       <c r="E274">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="G274">
         <v>0.4</v>
@@ -7552,7 +7549,7 @@
         <v>18</v>
       </c>
       <c r="E275">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="G275">
         <v>0.4</v>
@@ -7578,7 +7575,7 @@
         <v>18</v>
       </c>
       <c r="E276">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="G276">
         <v>0.4</v>
@@ -7604,7 +7601,7 @@
         <v>18</v>
       </c>
       <c r="E277">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="G277">
         <v>0.4</v>
@@ -7630,7 +7627,7 @@
         <v>18</v>
       </c>
       <c r="E278">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="G278">
         <v>0.4</v>
@@ -7656,7 +7653,7 @@
         <v>18</v>
       </c>
       <c r="E279">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="G279">
         <v>0.4</v>
@@ -7682,7 +7679,7 @@
         <v>18</v>
       </c>
       <c r="E280">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="G280">
         <v>0.4</v>
@@ -7708,7 +7705,7 @@
         <v>18</v>
       </c>
       <c r="E281">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="G281">
         <v>0.4</v>
@@ -7734,7 +7731,7 @@
         <v>18</v>
       </c>
       <c r="E282">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="G282">
         <v>0.4</v>
@@ -7760,7 +7757,7 @@
         <v>18</v>
       </c>
       <c r="E283">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="G283">
         <v>0.4</v>
@@ -7786,7 +7783,7 @@
         <v>18</v>
       </c>
       <c r="E284">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="G284">
         <v>0.4</v>
@@ -7812,7 +7809,7 @@
         <v>18</v>
       </c>
       <c r="E285">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="G285">
         <v>0.4</v>
@@ -7838,7 +7835,7 @@
         <v>18</v>
       </c>
       <c r="E286">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="G286">
         <v>0.4</v>
@@ -7864,7 +7861,7 @@
         <v>18</v>
       </c>
       <c r="E287">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="G287">
         <v>0.4</v>
@@ -7890,7 +7887,7 @@
         <v>18</v>
       </c>
       <c r="E288">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="G288">
         <v>0.4</v>
@@ -7916,7 +7913,7 @@
         <v>18</v>
       </c>
       <c r="E289">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="G289">
         <v>0.4</v>
@@ -7936,16 +7933,16 @@
         <v>19</v>
       </c>
       <c r="C290" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D290" t="s">
         <v>18</v>
       </c>
       <c r="E290">
-        <v>1990</v>
+        <v>2019</v>
       </c>
       <c r="G290">
-        <v>0.02</v>
+        <v>0.4</v>
       </c>
       <c r="I290" t="s">
         <v>45</v>
@@ -7968,7 +7965,7 @@
         <v>18</v>
       </c>
       <c r="E291">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="G291">
         <v>0.02</v>
@@ -7994,7 +7991,7 @@
         <v>18</v>
       </c>
       <c r="E292">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="G292">
         <v>0.02</v>
@@ -8020,7 +8017,7 @@
         <v>18</v>
       </c>
       <c r="E293">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="G293">
         <v>0.02</v>
@@ -8046,7 +8043,7 @@
         <v>18</v>
       </c>
       <c r="E294">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="G294">
         <v>0.02</v>
@@ -8072,7 +8069,7 @@
         <v>18</v>
       </c>
       <c r="E295">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="G295">
         <v>0.02</v>
@@ -8098,7 +8095,7 @@
         <v>18</v>
       </c>
       <c r="E296">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="G296">
         <v>0.02</v>
@@ -8124,7 +8121,7 @@
         <v>18</v>
       </c>
       <c r="E297">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="G297">
         <v>0.02</v>
@@ -8150,7 +8147,7 @@
         <v>18</v>
       </c>
       <c r="E298">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="G298">
         <v>0.02</v>
@@ -8176,7 +8173,7 @@
         <v>18</v>
       </c>
       <c r="E299">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="G299">
         <v>0.02</v>
@@ -8202,7 +8199,7 @@
         <v>18</v>
       </c>
       <c r="E300">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="G300">
         <v>0.02</v>
@@ -8228,7 +8225,7 @@
         <v>18</v>
       </c>
       <c r="E301">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="G301">
         <v>0.02</v>
@@ -8254,7 +8251,7 @@
         <v>18</v>
       </c>
       <c r="E302">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="G302">
         <v>0.02</v>
@@ -8280,7 +8277,7 @@
         <v>18</v>
       </c>
       <c r="E303">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="G303">
         <v>0.02</v>
@@ -8306,7 +8303,7 @@
         <v>18</v>
       </c>
       <c r="E304">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="G304">
         <v>0.02</v>
@@ -8332,7 +8329,7 @@
         <v>18</v>
       </c>
       <c r="E305">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="G305">
         <v>0.02</v>
@@ -8358,7 +8355,7 @@
         <v>18</v>
       </c>
       <c r="E306">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="G306">
         <v>0.02</v>
@@ -8384,7 +8381,7 @@
         <v>18</v>
       </c>
       <c r="E307">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="G307">
         <v>0.02</v>
@@ -8410,7 +8407,7 @@
         <v>18</v>
       </c>
       <c r="E308">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="G308">
         <v>0.02</v>
@@ -8436,7 +8433,7 @@
         <v>18</v>
       </c>
       <c r="E309">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="G309">
         <v>0.02</v>
@@ -8462,7 +8459,7 @@
         <v>18</v>
       </c>
       <c r="E310">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="G310">
         <v>0.02</v>
@@ -8488,7 +8485,7 @@
         <v>18</v>
       </c>
       <c r="E311">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="G311">
         <v>0.02</v>
@@ -8514,7 +8511,7 @@
         <v>18</v>
       </c>
       <c r="E312">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="G312">
         <v>0.02</v>
@@ -8540,7 +8537,7 @@
         <v>18</v>
       </c>
       <c r="E313">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="G313">
         <v>0.02</v>
@@ -8566,7 +8563,7 @@
         <v>18</v>
       </c>
       <c r="E314">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="G314">
         <v>0.02</v>
@@ -8592,7 +8589,7 @@
         <v>18</v>
       </c>
       <c r="E315">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="G315">
         <v>0.02</v>
@@ -8618,7 +8615,7 @@
         <v>18</v>
       </c>
       <c r="E316">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="G316">
         <v>0.02</v>
@@ -8644,7 +8641,7 @@
         <v>18</v>
       </c>
       <c r="E317">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="G317">
         <v>0.02</v>
@@ -8670,7 +8667,7 @@
         <v>18</v>
       </c>
       <c r="E318">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="G318">
         <v>0.02</v>
@@ -8696,7 +8693,7 @@
         <v>18</v>
       </c>
       <c r="E319">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="G319">
         <v>0.02</v>
@@ -8708,11 +8705,37 @@
         <v>46</v>
       </c>
     </row>
+    <row r="320" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A320" t="s">
+        <v>16</v>
+      </c>
+      <c r="B320" t="s">
+        <v>19</v>
+      </c>
+      <c r="C320" t="s">
+        <v>43</v>
+      </c>
+      <c r="D320" t="s">
+        <v>18</v>
+      </c>
+      <c r="E320">
+        <v>2019</v>
+      </c>
+      <c r="G320">
+        <v>0.02</v>
+      </c>
+      <c r="I320" t="s">
+        <v>45</v>
+      </c>
+      <c r="J320" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A5:L576" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A5:L577" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K10" r:id="rId1" xr:uid="{551E5581-983A-E74F-B049-6848A8895DFC}"/>
+    <hyperlink ref="K11" r:id="rId1" xr:uid="{551E5581-983A-E74F-B049-6848A8895DFC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>